<commit_message>
#update UI AP and export
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountPayable/AP_Standart_Report.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountPayable/AP_Standart_Report.xlsx
@@ -320,11 +320,11 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -332,8 +332,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -784,7 +784,7 @@
       <c r="O7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="P7" s="18" t="s">
+      <c r="P7" s="15" t="s">
         <v>46</v>
       </c>
       <c r="Q7" s="4" t="s">
@@ -822,7 +822,7 @@
       <c r="M8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="18" t="s">
         <v>36</v>
       </c>
       <c r="O8" s="7" t="s">
@@ -846,13 +846,13 @@
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="M9" s="15" t="s">
+      <c r="M9" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="N9" s="15" t="s">
+      <c r="N9" s="14" t="s">
         <v>42</v>
       </c>
       <c r="O9" s="10"/>

</xml_diff>

<commit_message>
#update AP theo CR trong task
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountPayable/AP_Standart_Report.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountPayable/AP_Standart_Report.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">BÁO CÁO CÔNG NỢ CHI TIẾT </t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>{PartnerCodeGrp}</t>
+  </si>
+  <si>
+    <t>{PartnerCodeDt}</t>
   </si>
 </sst>
 </file>
@@ -799,7 +802,9 @@
       <c r="B8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9" t="s">

</xml_diff>

<commit_message>
#commit #17167 AP Detail - Export - AP Account Template
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountPayable/AP_Standart_Report.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountPayable/AP_Standart_Report.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">BÁO CÁO CÔNG NỢ CHI TIẾT </t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>{PartnerCodeDt}</t>
+  </si>
+  <si>
+    <t>{DescriptionGrp}</t>
   </si>
 </sst>
 </file>
@@ -621,7 +624,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -638,7 +643,7 @@
     <col min="15" max="15" width="8.7109375" customWidth="1"/>
     <col min="16" max="16" width="14.42578125" customWidth="1"/>
     <col min="17" max="17" width="16.140625" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.2">
@@ -793,7 +798,9 @@
       <c r="Q7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="R7" s="4"/>
+      <c r="R7" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">

</xml_diff>